<commit_message>
include purity in models
</commit_message>
<xml_diff>
--- a/results/fgsea_R_pre_vs_post.xlsx
+++ b/results/fgsea_R_pre_vs_post.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -402,1980 +402,2910 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>GOBP_ANATOMICAL_STRUCTURE_FORMATION_INVOLVED_IN_MORPHOGENESIS</t>
+          <t>GOBP_ADAPTIVE_IMMUNE_RESPONSE</t>
         </is>
       </c>
       <c r="B2">
-        <v>0.00066282743326146</v>
+        <v>4.714305458980387e-11</v>
       </c>
       <c r="C2">
-        <v>0.02314480666742231</v>
+        <v>4.572876295210975e-09</v>
       </c>
       <c r="D2">
-        <v>0.4772708153628621</v>
+        <v>0.8513390571168989</v>
       </c>
       <c r="E2">
-        <v>0.4483026048828689</v>
+        <v>0.7407609123254623</v>
       </c>
       <c r="F2">
-        <v>2.351727139656173</v>
+        <v>3.762197722988711</v>
       </c>
       <c r="G2">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>THBS2,CTHRC1,CCL11,COL11A1,CYP1B1,FAP,APOLD1,C3,CHI3L1,COL1A1,COL12A1,CXCL10,SFRP2,WNT2,CALB1,HOPX,APELA,MMP2</t>
+          <t>IGKV3D-11,IGLL5,IGLV1-36,IGLV1-44,IGLV1-47,IGKC,IGKV1-16,IGKV1-5,IGKV1D-17,IGKV2-28,IGKV2D-28,CLC,JCHAIN,IGKV3-20,IGKV3D-20,IGKV1-12,IGKV1D-12,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,TNFRSF17,IGHG2,IGKV2-24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GOBP_ANIMAL_ORGAN_MORPHOGENESIS</t>
+          <t>GOBP_ANATOMICAL_STRUCTURE_FORMATION_INVOLVED_IN_MORPHOGENESIS</t>
         </is>
       </c>
       <c r="B3">
-        <v>0.1258581235697941</v>
+        <v>0.0004795140032172475</v>
       </c>
       <c r="C3">
-        <v>0.3611580937220177</v>
+        <v>0.002736050488945471</v>
       </c>
       <c r="D3">
-        <v>0.1900233052791083</v>
+        <v>0.4984931087665903</v>
       </c>
       <c r="E3">
-        <v>0.2676255666785606</v>
+        <v>-0.441500364840326</v>
       </c>
       <c r="F3">
-        <v>1.403922934126776</v>
+        <v>-2.370899925375345</v>
       </c>
       <c r="G3">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>SFRP4,ASPN,CTHRC1,CCL11,COL11A1,TNC,MMP13,COL1A1,SFRP2,WNT2,CALB1,COL1A2,MMP2,MYO7A,ID3,OVOL2,BMP2</t>
+          <t>ESM1,IL6,ANGPT2,FN1,GDF15,INHBA,COL4A1,SOX8,COL11A1,CXCL8,SERPINE1,THBS1,PTGS2,ACKR3,ENPEP,FLT1,ROBO4,MCAM,PDGFA,CALD1,COL4A2,ACTC1,WNT5A,ADAMTS5,IL1A</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GOBP_BIOLOGICAL_ADHESION</t>
+          <t>GOBP_ANIMAL_ORGAN_MORPHOGENESIS</t>
         </is>
       </c>
       <c r="B4">
-        <v>0.01513532469908418</v>
+        <v>0.01400678506097915</v>
       </c>
       <c r="C4">
-        <v>0.1427044900199366</v>
+        <v>0.02830537814406203</v>
       </c>
       <c r="D4">
         <v>0.3807304007227924</v>
       </c>
       <c r="E4">
-        <v>0.3341571993430477</v>
+        <v>-0.4024439415387129</v>
       </c>
       <c r="F4">
-        <v>1.827607507250685</v>
+        <v>-1.86118300753003</v>
       </c>
       <c r="G4">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>THBS2,CCL11,CEL,CYP1B1,SELE,FAP,TNC,FBLN1,PTPRO,CCDC80,COL1A1,COL12A1,LRRC15,REG3A,SFRP2</t>
+          <t>IL6,STC1,INHBA,SOX8,COL11A1,SERPINE1,TNFSF11,ACTG2,HAS2,SEMA3A,ID4,PDGFA,COL9A1,ACTC1,WNT5A,ADAMTS5,PTN</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GOBP_BIOLOGICAL_PROCESS_INVOLVED_IN_INTERSPECIES_INTERACTION_BETWEEN_ORGANISMS</t>
+          <t>GOBP_BIOLOGICAL_ADHESION</t>
         </is>
       </c>
       <c r="B5">
-        <v>0.1959459459459459</v>
+        <v>0.001958890655680297</v>
       </c>
       <c r="C5">
-        <v>0.4440835266821346</v>
+        <v>0.006155874011084922</v>
       </c>
       <c r="D5">
-        <v>0.1482615004751066</v>
+        <v>0.4317076958033464</v>
       </c>
       <c r="E5">
-        <v>0.2395489804931094</v>
+        <v>-0.4145668008553646</v>
       </c>
       <c r="F5">
-        <v>1.273570275967002</v>
+        <v>-2.150166399440014</v>
       </c>
       <c r="G5">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>CCL11,CXCL11,REG1B,SELE,UBD,FCGR3A,C3,CCDC80,LRRC15,CXCL10,REG3A,BST2</t>
+          <t>IL6,ANGPT2,FN1,NR4A3,CXCL8,SERPINE1,TESC,ITGA1,IBSP,THBS1,TNFSF11,SPP1,NTM,TNFSF4,ACKR3,HAS2,ROBO4,ANOS1,MCAM</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GOBP_BLOOD_VESSEL_MORPHOGENESIS</t>
+          <t>GOBP_BIOLOGICAL_PROCESS_INVOLVED_IN_INTERSPECIES_INTERACTION_BETWEEN_ORGANISMS</t>
         </is>
       </c>
       <c r="B6">
-        <v>0.07852193995381063</v>
+        <v>0.06463195691202872</v>
       </c>
       <c r="C6">
-        <v>0.3454965357967668</v>
+        <v>0.0940104671447955</v>
       </c>
       <c r="D6">
-        <v>0.2450417854309962</v>
+        <v>0.2377938344236881</v>
       </c>
       <c r="E6">
-        <v>0.350197451480241</v>
+        <v>0.2831435060124403</v>
       </c>
       <c r="F6">
-        <v>1.53743606884077</v>
+        <v>1.519171654711904</v>
       </c>
       <c r="G6">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>THBS2,CCL11,CYP1B1,FAP,APOLD1,C3,CHI3L1,CXCL10,SFRP2,APELA,MMP2</t>
+          <t>PLA2G2A,IGLL5,IGKC,REG1B,REG3A,REG1A,JCHAIN,CCL11,IGKV3-20,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,IGHG2,ITLN1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GOBP_CELLULAR_RESPONSE_TO_ENDOGENOUS_STIMULUS</t>
+          <t>GOBP_BLOOD_VESSEL_MORPHOGENESIS</t>
         </is>
       </c>
       <c r="B7">
-        <v>0.3055555555555556</v>
+        <v>0.0001550125761967252</v>
       </c>
       <c r="C7">
-        <v>0.5809859154929576</v>
+        <v>0.001074015706505882</v>
       </c>
       <c r="D7">
-        <v>0.09889030075206362</v>
+        <v>0.5188480777437918</v>
       </c>
       <c r="E7">
-        <v>-0.2430409883732239</v>
+        <v>-0.5063131231392576</v>
       </c>
       <c r="F7">
-        <v>-1.107481365063664</v>
+        <v>-2.551653609943905</v>
       </c>
       <c r="G7">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>SLC26A3,CA2,AQP8,BAMBI</t>
+          <t>ESM1,IL6,ANGPT2,FN1,COL4A1,CXCL8,SERPINE1,ADGRF5,THBS1,PTGS2,ACKR3,HAS2,ENPEP,FLT1,ROBO4,LOX,MCAM,PDGFA,CALD1,COL4A2</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GOBP_CELLULAR_RESPONSE_TO_OXYGEN_CONTAINING_COMPOUND</t>
+          <t>GOBP_B_CELL_ACTIVATION</t>
         </is>
       </c>
       <c r="B8">
-        <v>0.2413194444444444</v>
+        <v>0.07582535384286707</v>
       </c>
       <c r="C8">
-        <v>0.4977213541666667</v>
+        <v>0.1021536017049737</v>
       </c>
       <c r="D8">
-        <v>0.11378726182188</v>
+        <v>0.2878051305355643</v>
       </c>
       <c r="E8">
-        <v>-0.2618660709122733</v>
+        <v>0.3790070715775362</v>
       </c>
       <c r="F8">
-        <v>-1.193262896184525</v>
+        <v>1.615474297785913</v>
       </c>
       <c r="G8">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>SLC26A3,CA2,AQP8,NEUROD1</t>
+          <t>IGLL5,IGKC,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,IGHG2,MZB1,POU2AF1,MS4A1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GOBP_CELL_CELL_SIGNALING</t>
+          <t>GOBP_CELLULAR_RESPONSE_TO_ENDOGENOUS_STIMULUS</t>
         </is>
       </c>
       <c r="B9">
-        <v>0.1133333333333333</v>
+        <v>0.0002205451189677553</v>
       </c>
       <c r="C9">
-        <v>0.3611580937220177</v>
+        <v>0.001337054783742017</v>
       </c>
       <c r="D9">
-        <v>0.1978220213151033</v>
+        <v>0.5188480777437918</v>
       </c>
       <c r="E9">
-        <v>0.2573794675693324</v>
+        <v>-0.4998067696025833</v>
       </c>
       <c r="F9">
-        <v>1.407686705738135</v>
+        <v>-2.498947387390903</v>
       </c>
       <c r="G9">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>FAM3B,SFRP4,CTHRC1,CEL,CXCL11,GABBR1,TNC,C3,PTPRO,COL1A1,CXCL10,SFRP2,WNT2,CALB1</t>
+          <t>STC1,GDF15,BMP8A,INHBA,COL4A1,NR4A3,CXCL8,ANO1,THBS1,CA2,PTGS2,DKK3,TNFSF4,MAP1B,HAS2,LOX,PDGFA,COL4A2,LPL,CAV2,WNT5A</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>GOBP_CELL_MIGRATION</t>
+          <t>GOBP_CELLULAR_RESPONSE_TO_LIPID</t>
         </is>
       </c>
       <c r="B10">
-        <v>0.1222222222222222</v>
+        <v>0.008835439635894659</v>
       </c>
       <c r="C10">
-        <v>0.3611580937220177</v>
+        <v>0.01896100130560613</v>
       </c>
       <c r="D10">
-        <v>0.1900233052791083</v>
+        <v>0.3807304007227924</v>
       </c>
       <c r="E10">
-        <v>0.2538349388489948</v>
+        <v>-0.4518083856945838</v>
       </c>
       <c r="F10">
-        <v>1.3883005985057</v>
+        <v>-1.906892715871385</v>
       </c>
       <c r="G10">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>MMP7,CTHRC1,CCL11,CXCL11,CYP1B1,SELE,FAP,PTPRO,COL1A1,LRRC15,CXCL10,SFRP2,BST2</t>
+          <t>IL6,STC1,INHBA,NR4A3,CXCL8,SERPINE1,TESC,SPP1,CXCL5,TNFSF4</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>GOBP_CHEMICAL_HOMEOSTASIS</t>
+          <t>GOBP_CELLULAR_RESPONSE_TO_OXYGEN_CONTAINING_COMPOUND</t>
         </is>
       </c>
       <c r="B11">
-        <v>0.1571753986332574</v>
+        <v>7.963352154209159e-05</v>
       </c>
       <c r="C11">
-        <v>0.4083526682134571</v>
+        <v>0.0009003292979184316</v>
       </c>
       <c r="D11">
-        <v>0.1682381656896396</v>
+        <v>0.5384340963099162</v>
       </c>
       <c r="E11">
-        <v>0.3067326099619792</v>
+        <v>-0.5198246516995744</v>
       </c>
       <c r="F11">
-        <v>1.30832308815593</v>
+        <v>-2.619747323203851</v>
       </c>
       <c r="G11">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>FAM3B,SFRP4,CCL11,CXCL11</t>
+          <t>IL6,MMP3,STC1,GDF15,INHBA,COL4A1,NR4A3,CXCL8,SERPINE1,TESC,ANO1,CA2,SPP1,PTGS2,CXCL5,TNFSF4,MAP1B</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>GOBP_CIRCULATORY_SYSTEM_DEVELOPMENT</t>
+          <t>GOBP_CELLULAR_RESPONSE_TO_STRESS</t>
         </is>
       </c>
       <c r="B12">
-        <v>0.006547888844985692</v>
+        <v>0.00611850897278895</v>
       </c>
       <c r="C12">
-        <v>0.08643213275381112</v>
+        <v>0.01447549683806166</v>
       </c>
       <c r="D12">
         <v>0.4070179189239539</v>
       </c>
       <c r="E12">
-        <v>0.3742726923989185</v>
+        <v>-0.4337766369065549</v>
       </c>
       <c r="F12">
-        <v>1.989833457709558</v>
+        <v>-2.041350971463878</v>
       </c>
       <c r="G12">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>THBS2,CCL11,COL11A1,CYP1B1,FAP,APOLD1,C3,CHI3L1,COL1A1,NOX4,CXCL10,SFRP2,WNT2,HOPX,COL1A2,APELA,MMP2</t>
+          <t>IL6,MMP3,STC1,NR4A3,CXCL8,ANO1,THBS1,TNFSF11,SPP1,PTGS2,MAP1B,ACKR3,HAS2,SEMA3A,IER3</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>GOBP_DEFENSE_RESPONSE</t>
+          <t>GOBP_CELL_ACTIVATION</t>
         </is>
       </c>
       <c r="B13">
-        <v>0.3482142857142857</v>
+        <v>0.6873857404021938</v>
       </c>
       <c r="C13">
-        <v>0.5809859154929576</v>
+        <v>0.6945460085313834</v>
       </c>
       <c r="D13">
-        <v>0.1063232559327084</v>
+        <v>0.05884381695958071</v>
       </c>
       <c r="E13">
-        <v>0.2015807316474434</v>
+        <v>0.1623794945320692</v>
       </c>
       <c r="F13">
-        <v>1.083152901897141</v>
+        <v>0.8107654139954666</v>
       </c>
       <c r="G13">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>CCL11,CXCL11,SELE,UBD,FCGR3A,C3,CHI3L1,NOX4,MMP3,CXCL10,REG3A,BST2</t>
+          <t>PLA2G2A,IGLL5,IGKC,CLC,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,IGHG2,MZB1,POU2AF1,MS4A1</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>GOBP_EMBRYO_DEVELOPMENT</t>
+          <t>GOBP_CELL_CELL_SIGNALING</t>
         </is>
       </c>
       <c r="B14">
-        <v>0.07852193995381063</v>
+        <v>0.004359465834982573</v>
       </c>
       <c r="C14">
-        <v>0.3454965357967668</v>
+        <v>0.01174633849981416</v>
       </c>
       <c r="D14">
-        <v>0.2450417854309962</v>
+        <v>0.4070179189239539</v>
       </c>
       <c r="E14">
-        <v>0.3502861582339521</v>
+        <v>-0.4322122372525473</v>
       </c>
       <c r="F14">
-        <v>1.537825509032664</v>
+        <v>-2.095303199564562</v>
       </c>
       <c r="G14">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>CTHRC1,COL11A1,COL1A1,COL12A1,SFRP2,WNT2,HOPX,APELA,MMP2,MYO7A,ID3,OVOL2,BMP2</t>
+          <t>IL6,IL11,GDF15,BMP8A,INHBA,ANO1,CA2,TNFSF11,SPP1,PTGS2,DKK3,CXCL5,MAP1B,ENPEP</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>GOBP_EPITHELIUM_DEVELOPMENT</t>
+          <t>GOBP_CELL_MIGRATION</t>
         </is>
       </c>
       <c r="B15">
-        <v>0.108167770419426</v>
+        <v>5.108661554863162e-05</v>
       </c>
       <c r="C15">
-        <v>0.3611580937220177</v>
+        <v>0.0007079145297453238</v>
       </c>
       <c r="D15">
-        <v>0.2020717090211599</v>
+        <v>0.557332238758646</v>
       </c>
       <c r="E15">
-        <v>0.260438843763246</v>
+        <v>-0.4913575276206097</v>
       </c>
       <c r="F15">
-        <v>1.409376241019202</v>
+        <v>-2.664290890809203</v>
       </c>
       <c r="G15">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>SFRP4,CTHRC1,CCL11,APOLD1,TNC,C3,PTPRO,CXCL10,REG3A,SFRP2,WNT2,CALB1,APELA,MMP2,MYO7A,ID3,OVOL2,BMP2,PLA2G10,SPINK5,DHRS9,KLF4</t>
+          <t>IL6,ANGPT2,FN1,STC1,NR4A3,SOX8,CXCL8,SERPINE1,ITGA1,THBS1,TNFSF11,PTGS2,CXCL5,MAP1B,ACKR3,HAS2,ENPEP,FLT1,SEMA3A,ROBO4,LOX,MCAM,PDGFA,IL24,WNT5A,RHOBTB3,PTN,IL1A</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GOBP_EXTERNAL_ENCAPSULATING_STRUCTURE_ORGANIZATION</t>
+          <t>GOBP_CELL_MORPHOGENESIS</t>
         </is>
       </c>
       <c r="B16">
-        <v>0.0007013577778006761</v>
+        <v>0.01587237248305408</v>
       </c>
       <c r="C16">
-        <v>0.02314480666742231</v>
+        <v>0.03140213343556689</v>
       </c>
       <c r="D16">
-        <v>0.4772708153628621</v>
+        <v>0.3524878575836192</v>
       </c>
       <c r="E16">
-        <v>0.4795263034239414</v>
+        <v>-0.4266722617691489</v>
       </c>
       <c r="F16">
-        <v>2.271199051740747</v>
+        <v>-1.800803734045684</v>
       </c>
       <c r="G16">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>MMP7,COL11A1,CYP1B1,FAP,MMP13,FBLN1,CCDC80,COL1A1,COL12A1,MMP3,SFRP2,COL1A2,MMP11,MMP1,MMP2</t>
+          <t>FN1,STC1,COCH,ITGA1,SPP1,MAP1B,HAS2,SEMA3A,ROBO4,ANOS1,HECW2,WNT5A,RHOBTB3,PTN</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>GOBP_HOMEOSTATIC_PROCESS</t>
+          <t>GOBP_CHEMICAL_HOMEOSTASIS</t>
         </is>
       </c>
       <c r="B17">
-        <v>0.3163972286374134</v>
+        <v>0.2563025210084033</v>
       </c>
       <c r="C17">
-        <v>0.5809859154929576</v>
+        <v>0.2857625808944267</v>
       </c>
       <c r="D17">
-        <v>0.1147507192270233</v>
+        <v>0.1226791895688083</v>
       </c>
       <c r="E17">
-        <v>0.2314616921587931</v>
+        <v>-0.2793354916552652</v>
       </c>
       <c r="F17">
-        <v>1.122455483318433</v>
+        <v>-1.178957343837018</v>
       </c>
       <c r="G17">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>FAM3B,SFRP4,CCL11,CXCL11</t>
+          <t>IL6,STC1,ANO1,ADGRF5,CA2,TNFSF11,ACKR3,HAS2,LPL,CAV2,WNT5A,IL1A</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>GOBP_IMMUNE_RESPONSE</t>
+          <t>GOBP_CIRCULATORY_SYSTEM_DEVELOPMENT</t>
         </is>
       </c>
       <c r="B18">
-        <v>0.09237875288683603</v>
+        <v>0.000121260598032923</v>
       </c>
       <c r="C18">
-        <v>0.3586469229724222</v>
+        <v>0.001069298000835776</v>
       </c>
       <c r="D18">
-        <v>0.2249660935403137</v>
+        <v>0.5384340963099162</v>
       </c>
       <c r="E18">
-        <v>0.3198325707674355</v>
+        <v>-0.4888997286998304</v>
       </c>
       <c r="F18">
-        <v>1.477929799509988</v>
+        <v>-2.535696942390874</v>
       </c>
       <c r="G18">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>CCL11,CXCL11,REG1B,UBD,FCGR3A,C3,CXCL10,REG3A,BST2,CLC,IFI44</t>
+          <t>ESM1,IL6,ANGPT2,FN1,COL4A1,COL11A1,CXCL8,SERPINE1,ADGRF5,THBS1,PTGS2,ACKR3,HAS2,ENPEP,FLT1,ROBO4,LOX,MCAM,PDGFA,CALD1,COL4A2</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>GOBP_INFLAMMATORY_RESPONSE</t>
+          <t>GOBP_CYTOKINE_PRODUCTION</t>
         </is>
       </c>
       <c r="B19">
-        <v>0.1200923787528868</v>
+        <v>0.4762931034482759</v>
       </c>
       <c r="C19">
-        <v>0.3611580937220177</v>
+        <v>0.4967788283277716</v>
       </c>
       <c r="D19">
-        <v>0.1957890021489494</v>
+        <v>0.0857844408075645</v>
       </c>
       <c r="E19">
-        <v>0.3106579874298717</v>
+        <v>-0.2305517042374308</v>
       </c>
       <c r="F19">
-        <v>1.435534523506241</v>
+        <v>-0.9781144714230905</v>
       </c>
       <c r="G19">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>CCL11,CXCL11,SELE,FCGR3A,C3,CHI3L1,NOX4,MMP3,CXCL10,REG3A</t>
+          <t>IL6,FN1,INHBA,NR4A3,SERPINE1,THBS1,PTGS2,TNFSF4</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>GOBP_LIPID_METABOLIC_PROCESS</t>
+          <t>GOBP_DEFENSE_RESPONSE</t>
         </is>
       </c>
       <c r="B20">
-        <v>0.6571936056838366</v>
+        <v>0.196113074204947</v>
       </c>
       <c r="C20">
-        <v>0.8674955595026643</v>
+        <v>0.2264639071176174</v>
       </c>
       <c r="D20">
-        <v>0.05960370425759728</v>
+        <v>0.1294428877450463</v>
       </c>
       <c r="E20">
-        <v>-0.2008731354395721</v>
+        <v>0.2294778279459622</v>
       </c>
       <c r="F20">
-        <v>-0.8284158980682748</v>
+        <v>1.250447216385486</v>
       </c>
       <c r="G20">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>CWH43,SDR16C5,SPTSSB,FUT3,VSIG2</t>
+          <t>PLA2G2A,IGLL5,IGKC,ORM1,ORM2,REG3A,JCHAIN,CCL11,IGKV3-20,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,IGHG2</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>GOBP_LOCOMOTION</t>
+          <t>GOBP_DEFENSE_RESPONSE_TO_BACTERIUM</t>
         </is>
       </c>
       <c r="B21">
-        <v>0.08577878103837472</v>
+        <v>0.005059645486202018</v>
       </c>
       <c r="C21">
-        <v>0.3538374717832957</v>
+        <v>0.01291541084635778</v>
       </c>
       <c r="D21">
-        <v>0.2311267096738343</v>
+        <v>0.4070179189239539</v>
       </c>
       <c r="E21">
-        <v>0.2596841843927877</v>
+        <v>0.4860775355674358</v>
       </c>
       <c r="F21">
-        <v>1.450689317735771</v>
+        <v>2.071849905522587</v>
       </c>
       <c r="G21">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>MMP7,CTHRC1,CCL11,CXCL11,CYP1B1,SELE,FAP,FBLN1,PTPRO,COL1A1,LRRC15,CXCL10,SFRP2,BST2</t>
+          <t>PLA2G2A,IGLL5,IGKC,JCHAIN,IGKV3-20,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,IGHG2</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>GOBP_MORPHOGENESIS_OF_AN_EPITHELIUM</t>
+          <t>GOBP_DEFENSE_RESPONSE_TO_OTHER_ORGANISM</t>
         </is>
       </c>
       <c r="B22">
-        <v>0.8906605922551253</v>
+        <v>0.006517352699972982</v>
       </c>
       <c r="C22">
-        <v>0.9567579006772009</v>
+        <v>0.01505198123565189</v>
       </c>
       <c r="D22">
-        <v>0.05700595265823873</v>
+        <v>0.4070179189239539</v>
       </c>
       <c r="E22">
-        <v>0.1490491140093783</v>
+        <v>0.4371236978767231</v>
       </c>
       <c r="F22">
-        <v>0.6357471973776339</v>
+        <v>1.964357755904153</v>
       </c>
       <c r="G22">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>CTHRC1,CCL11,TNC,CXCL10,SFRP2,WNT2,MMP2,OVOL2,BMP2,PLA2G10</t>
+          <t>PLA2G2A,IGLL5,IGKC,JCHAIN,CCL11,IGKV3-20,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,IGHG2</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>GOBP_NEGATIVE_REGULATION_OF_CATALYTIC_ACTIVITY</t>
+          <t>GOBP_ENDOCYTOSIS</t>
         </is>
       </c>
       <c r="B23">
-        <v>0.9179954441913439</v>
+        <v>0.1007604562737643</v>
       </c>
       <c r="C23">
-        <v>0.9567579006772009</v>
+        <v>0.1286021612967781</v>
       </c>
       <c r="D23">
-        <v>0.05559470977588687</v>
+        <v>0.1938133027253105</v>
       </c>
       <c r="E23">
-        <v>0.1404148687998334</v>
+        <v>0.3370536515610452</v>
       </c>
       <c r="F23">
-        <v>0.5989190871944762</v>
+        <v>1.411594046806142</v>
       </c>
       <c r="G23">
         <v>15</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>GABBR1,C3,PTPRO,SFRP2,BST2,SPOCK1,BMP2,TFPI2,SPINK5,PI3,KLF4</t>
+          <t>IGLL5,IGKC,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,IGHG2</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>GOBP_NEGATIVE_REGULATION_OF_DEVELOPMENTAL_PROCESS</t>
+          <t>GOBP_ENZYME_LINKED_RECEPTOR_PROTEIN_SIGNALING_PATHWAY</t>
         </is>
       </c>
       <c r="B24">
-        <v>0.1643192488262911</v>
+        <v>0.001895118645380043</v>
       </c>
       <c r="C24">
-        <v>0.4083526682134571</v>
+        <v>0.006155874011084922</v>
       </c>
       <c r="D24">
-        <v>0.1669338487131931</v>
+        <v>0.4550598673872295</v>
       </c>
       <c r="E24">
-        <v>0.2817799484877151</v>
+        <v>-0.4764910311130967</v>
       </c>
       <c r="F24">
-        <v>1.334605312024064</v>
+        <v>-2.151723777217885</v>
       </c>
       <c r="G24">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>ASPN,THBS2,CCL11,FBLN1,CXCL10,REG3A,SFRP2,HOPX,MMP11,ID3,OVOL2,BMP2,SPINK5,PLAC8,KLF4,ID4,ADGRV1</t>
+          <t>ESM1,ANGPT2,GDF15,BMP8A,INHBA,COL4A1,NR4A3,ITGA1,THBS1,DKK3,FLT1,LOX,PDGFA,COL4A2,CAV2,WNT5A,PTN</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>GOBP_NEGATIVE_REGULATION_OF_MOLECULAR_FUNCTION</t>
+          <t>GOBP_EPITHELIUM_DEVELOPMENT</t>
         </is>
       </c>
       <c r="B25">
-        <v>0.352112676056338</v>
+        <v>0.09725158562367865</v>
       </c>
       <c r="C25">
-        <v>0.5809859154929576</v>
+        <v>0.1257787174066244</v>
       </c>
       <c r="D25">
-        <v>0.1088201267691612</v>
+        <v>0.2089550275493539</v>
       </c>
       <c r="E25">
-        <v>0.2305219721730415</v>
+        <v>-0.3198751117060044</v>
       </c>
       <c r="F25">
-        <v>1.091830168369193</v>
+        <v>-1.419502203211409</v>
       </c>
       <c r="G25">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>SFRP4,CYP1B1,GABBR1,C3,PTPRO,SFRP2,BST2,SPOCK1,ID3,BMP2,TFPI2,PLA2G10,SPINK5,PI3,KLF4</t>
+          <t>STC1,INHBA,COL4A1,SOX8,SERPINE1,CA2,TNFSF11,MAP1B,SEMA3A,ROBO4,ID4</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>GOBP_NEGATIVE_REGULATION_OF_MULTICELLULAR_ORGANISMAL_PROCESS</t>
+          <t>GOBP_EXTERNAL_ENCAPSULATING_STRUCTURE_ORGANIZATION</t>
         </is>
       </c>
       <c r="B26">
-        <v>0.2124711316397229</v>
+        <v>0.00155777109837144</v>
       </c>
       <c r="C26">
-        <v>0.4523578931684422</v>
+        <v>0.005396564162215346</v>
       </c>
       <c r="D26">
-        <v>0.1437589890392754</v>
+        <v>0.4550598673872295</v>
       </c>
       <c r="E26">
-        <v>0.2530285092658265</v>
+        <v>-0.4811124466077906</v>
       </c>
       <c r="F26">
-        <v>1.227042086370258</v>
+        <v>-2.172593025440893</v>
       </c>
       <c r="G26">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>ASPN,THBS2,CCL11,FAP,PTPRO,CXCL10,REG3A,SFRP2,BST2,MMP2,OVOL2,BMP2,PLA2G10,SPINK5,PLAC8,KLF4</t>
+          <t>COL10A1,MMP10,IL6,ADAMTS4,MMP3,COL4A1,MMP1,COL11A1,IBSP,HAS2,LOX,COL4A2,COL9A1,NID2,CAV2,PXDN,ADAMTS5</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>GOBP_NEGATIVE_REGULATION_OF_PROTEIN_METABOLIC_PROCESS</t>
+          <t>GOBP_HOMEOSTATIC_PROCESS</t>
         </is>
       </c>
       <c r="B27">
-        <v>0.7202797202797203</v>
+        <v>0.7724137931034483</v>
       </c>
       <c r="C27">
-        <v>0.9142011834319527</v>
+        <v>0.7724137931034483</v>
       </c>
       <c r="D27">
-        <v>0.06831108583186465</v>
+        <v>0.06421408818446053</v>
       </c>
       <c r="E27">
-        <v>0.1820306017953889</v>
+        <v>-0.1398638299002477</v>
       </c>
       <c r="F27">
-        <v>0.8093737522636224</v>
+        <v>-0.7583844899281597</v>
       </c>
       <c r="G27">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>IGF2BP3,C3,FBLN1,PTPRO,SFRP2,BST2,GAS1,SPOCK1,BMP2,TFPI2,SPINK5,PI3,KLF4</t>
+          <t>IL6,STC1,BMP8A,INHBA,NR4A3,ANO1,ADGRF5,CA2,TNFSF11,SPP1,PTGS2,ACKR3,HAS2</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>GOBP_NEGATIVE_REGULATION_OF_RESPONSE_TO_STIMULUS</t>
+          <t>GOBP_HUMORAL_IMMUNE_RESPONSE</t>
         </is>
       </c>
       <c r="B28">
-        <v>0.2009237875288684</v>
+        <v>0.0006158442096284453</v>
       </c>
       <c r="C28">
-        <v>0.4440835266821346</v>
+        <v>0.002844613730188533</v>
       </c>
       <c r="D28">
-        <v>0.1482615004751066</v>
+        <v>0.4772708153628621</v>
       </c>
       <c r="E28">
-        <v>0.2832538601960994</v>
+        <v>0.5170224964230159</v>
       </c>
       <c r="F28">
-        <v>1.243540463995739</v>
+        <v>2.323409039040251</v>
       </c>
       <c r="G28">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>SFRP4,ASPN,CTHRC1,FAP,FBLN1,PTPRO</t>
+          <t>IGLL5,IGKC,REG1B,REG3A,REG1A,JCHAIN,IGKV3-20,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,IGHG2,POU2AF1,MS4A1</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>GOBP_NEUROGENESIS</t>
+          <t>GOBP_IMMUNE_EFFECTOR_PROCESS</t>
         </is>
       </c>
       <c r="B29">
-        <v>0.8941441441441441</v>
+        <v>0.03213739668425034</v>
       </c>
       <c r="C29">
-        <v>0.9567579006772009</v>
+        <v>0.05152785905062243</v>
       </c>
       <c r="D29">
-        <v>0.05629407497009682</v>
+        <v>0.3217759180753611</v>
       </c>
       <c r="E29">
-        <v>0.1203218666713297</v>
+        <v>0.4192520503788618</v>
       </c>
       <c r="F29">
-        <v>0.6396952833029406</v>
+        <v>1.787013917344647</v>
       </c>
       <c r="G29">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>CTHRC1,CCL11,C3,PTPRO,BHLHE22,SFRP2,WNT2,MMP2,SPOCK1,MYO7A,STMN2,ID3,BMP2,PLA2G10,SPINK5,KLF4,ID4,HES2,ADGRV1</t>
+          <t>IGLL5,IGKC,CLC,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,IGHG2,MZB1,POU2AF1</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>GOBP_NEURON_DIFFERENTIATION</t>
+          <t>GOBP_IMMUNE_RESPONSE</t>
         </is>
       </c>
       <c r="B30">
-        <v>0.927765237020316</v>
+        <v>1.909602189988341e-07</v>
       </c>
       <c r="C30">
-        <v>0.9567579006772009</v>
+        <v>9.261570621443454e-06</v>
       </c>
       <c r="D30">
-        <v>0.05468084887854419</v>
+        <v>0.6901324587967956</v>
       </c>
       <c r="E30">
-        <v>0.1266204297433734</v>
+        <v>0.5481989884886305</v>
       </c>
       <c r="F30">
-        <v>0.6389687952412046</v>
+        <v>3.182063153066573</v>
       </c>
       <c r="G30">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>CTHRC1,C3,PTPRO,BHLHE22,SFRP2,WNT2,MMP2,SPOCK1,MYO7A,STMN2,ID3,BMP2,PLA2G10,SPINK5,KLF4,ID4,ADGRV1</t>
+          <t>IGKV3D-11,IGLL5,IGLV1-36,IGLV1-44,IGLV1-47,IGKC,IGKV1-16,IGKV1-5,IGKV1D-17,REG1B,REG3A,REG1A,IGKV2-28,IGKV2D-28,CLC,JCHAIN,CCL11,IGKV3-20,IGKV3D-20,IGKV1-12,IGKV1D-12,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,TNFRSF17,IGHG2,IGKV2-24</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>GOBP_NITROGEN_COMPOUND_TRANSPORT</t>
+          <t>GOBP_IMMUNE_SYSTEM_DEVELOPMENT</t>
         </is>
       </c>
       <c r="B31">
-        <v>0.4833040421792619</v>
+        <v>0.1134453781512605</v>
       </c>
       <c r="C31">
-        <v>0.7214780600461893</v>
+        <v>0.1392936921604085</v>
       </c>
       <c r="D31">
-        <v>0.07417589655880091</v>
+        <v>0.191892240384838</v>
       </c>
       <c r="E31">
-        <v>-0.2303975635389365</v>
+        <v>-0.3331217876730334</v>
       </c>
       <c r="F31">
-        <v>-0.9786299670451505</v>
+        <v>-1.405966623295847</v>
       </c>
       <c r="G31">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>CA2,ZG16,NEUROD1,PCSK1,CHGA,NTRK2,SLC6A14,MLPH,FFAR4</t>
+          <t>IL6,IL11,INHBA,TESC,ADGRF5,TNFSF11,TNFSF4,FLT1,LOX,WNT5A,PTN,IL1A,MS4A1,POU2AF1</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>GOBP_OSSIFICATION</t>
+          <t>GOBP_IMMUNOGLOBULIN_PRODUCTION</t>
         </is>
       </c>
       <c r="B32">
-        <v>0.1468531468531468</v>
+        <v>6.471313801154594e-06</v>
       </c>
       <c r="C32">
-        <v>0.4038461538461539</v>
+        <v>0.0001572205087683106</v>
       </c>
       <c r="D32">
-        <v>0.176694268938498</v>
+        <v>0.610526878385931</v>
       </c>
       <c r="E32">
-        <v>0.3070492910494734</v>
+        <v>0.6498542869863526</v>
       </c>
       <c r="F32">
-        <v>1.36525196519398</v>
+        <v>2.864288708220476</v>
       </c>
       <c r="G32">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>ASPN,CTHRC1,COL11A1,GABBR1,TNC,MMP13</t>
+          <t>IGKV3D-11,IGLV1-36,IGLV1-44,IGLV1-47,IGKC,IGKV1-16,IGKV1-5,IGKV1D-17,IGKV2-28,IGKV2D-28,IGKV3-20,IGKV3D-20,IGKV1-12,IGKV1D-12</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>GOBP_PHOSPHORYLATION</t>
+          <t>GOBP_INFLAMMATORY_RESPONSE</t>
         </is>
       </c>
       <c r="B33">
-        <v>0.6127562642369021</v>
+        <v>0.2678185745140389</v>
       </c>
       <c r="C33">
-        <v>0.82534517223746</v>
+        <v>0.2952091105438838</v>
       </c>
       <c r="D33">
-        <v>0.07530937641727728</v>
+        <v>0.1215432820354691</v>
       </c>
       <c r="E33">
-        <v>0.2036934499194726</v>
+        <v>-0.2423421450914306</v>
       </c>
       <c r="F33">
-        <v>0.8688246204693172</v>
+        <v>-1.174840109172363</v>
       </c>
       <c r="G33">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>CCL11,C3,FBLN1,PTPRO,CHI3L1,NOX4,SFRP2</t>
+          <t>IL6,FN1,MMP3,CXCL8,SERPINE1,THBS1,TNFSF11,SPP1,PTGS2,CXCL5,TNFSF4</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>GOBP_POSITIVE_REGULATION_OF_CELLULAR_BIOSYNTHETIC_PROCESS</t>
+          <t>GOBP_LOCOMOTION</t>
         </is>
       </c>
       <c r="B34">
-        <v>0.8324607329842932</v>
+        <v>2.37566351801543e-05</v>
       </c>
       <c r="C34">
-        <v>0.9567579006772009</v>
+        <v>0.0004608787224949933</v>
       </c>
       <c r="D34">
-        <v>0.04782996331142293</v>
+        <v>0.5756102610711286</v>
       </c>
       <c r="E34">
-        <v>-0.1609748096283872</v>
+        <v>-0.4989582792043604</v>
       </c>
       <c r="F34">
-        <v>-0.7029578173898251</v>
+        <v>-2.732657109233276</v>
       </c>
       <c r="G34">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>NEUROD1,BAMBI,SOX8,PKIB,ID4,GCG,KLF4,PLAC8,BMP2,OVOL2,GLYR1,WNT2,SFRP2,CXCL10,NOX4,COL1A1</t>
+          <t>IL6,ANGPT2,FN1,STC1,NR4A3,SOX8,CXCL8,SERPINE1,ITGA1,THBS1,TNFSF11,PTGS2,CXCL5,MAP1B,ACKR3,HAS2,ENPEP,FLT1,SEMA3A,ROBO4,ANOS1,LOX,MCAM,PDGFA,IL24,WNT5A,RHOBTB3,PTN,IL1A</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>GOBP_POSITIVE_REGULATION_OF_CELL_POPULATION_PROLIFERATION</t>
+          <t>GOBP_LYMPHOCYTE_ACTIVATION</t>
         </is>
       </c>
       <c r="B35">
-        <v>0.2655889145496536</v>
+        <v>0.074487895716946</v>
       </c>
       <c r="C35">
-        <v>0.5311778290993071</v>
+        <v>0.1017651533034333</v>
       </c>
       <c r="D35">
-        <v>0.1268757299298574</v>
+        <v>0.2249660935403137</v>
       </c>
       <c r="E35">
-        <v>0.2425573809237331</v>
+        <v>0.3296693787257705</v>
       </c>
       <c r="F35">
-        <v>1.176263163454364</v>
+        <v>1.481476763052784</v>
       </c>
       <c r="G35">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>CTHRC1,CCL11,REG1B,TNC,FCGR3A,CXCL10,REG3A,SFRP2,BST2,WNT2,APELA,MMP2</t>
+          <t>IGLL5,IGKC,CLC,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,IGHG2,MZB1,POU2AF1,MS4A1</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>GOBP_POSITIVE_REGULATION_OF_DEVELOPMENTAL_PROCESS</t>
+          <t>GOBP_MAPK_CASCADE</t>
         </is>
       </c>
       <c r="B36">
-        <v>0.1241534988713318</v>
+        <v>0.09267241379310345</v>
       </c>
       <c r="C36">
-        <v>0.3611580937220177</v>
+        <v>0.1214760018639329</v>
       </c>
       <c r="D36">
-        <v>0.1900233052791083</v>
+        <v>0.2165428367353482</v>
       </c>
       <c r="E36">
-        <v>0.2739948682839481</v>
+        <v>-0.3336683960879477</v>
       </c>
       <c r="F36">
-        <v>1.382669220476479</v>
+        <v>-1.415586529492966</v>
       </c>
       <c r="G36">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>SFRP4,THBS2,CTHRC1,CCL11,CYP1B1,C3,CHI3L1,COL1A1,SFRP2,WNT2,HOPX,APELA</t>
+          <t>IL6,FN1,IL11,GDF15,ITGA1,THBS1,TNFSF11,ACKR3,FLT1,SEMA3A,PDGFA,CAV2,WNT5A,IL1A</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>GOBP_POSITIVE_REGULATION_OF_GENE_EXPRESSION</t>
+          <t>GOBP_MULTICELLULAR_ORGANISMAL_HOMEOSTASIS</t>
         </is>
       </c>
       <c r="B37">
-        <v>0.8507992895204263</v>
+        <v>0.4600840336134454</v>
       </c>
       <c r="C37">
-        <v>0.9567579006772009</v>
+        <v>0.4850886006576544</v>
       </c>
       <c r="D37">
-        <v>0.04763872592908251</v>
+        <v>0.08628656262672446</v>
       </c>
       <c r="E37">
-        <v>-0.1610381016959322</v>
+        <v>-0.2315011952532831</v>
       </c>
       <c r="F37">
-        <v>-0.6641332269131531</v>
+        <v>-0.9770689454232875</v>
       </c>
       <c r="G37">
         <v>15</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>ORM2,ORM1</t>
+          <t>IL6,BMP8A,NR4A3,ADGRF5,TNFSF11,SPP1,PTGS2</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>GOBP_POSITIVE_REGULATION_OF_MOLECULAR_FUNCTION</t>
+          <t>GOBP_NEGATIVE_REGULATION_OF_CELL_POPULATION_PROLIFERATION</t>
         </is>
       </c>
       <c r="B38">
-        <v>0.4919168591224019</v>
+        <v>0.02103366353768697</v>
       </c>
       <c r="C38">
-        <v>0.7214780600461893</v>
+        <v>0.03709573387555702</v>
       </c>
       <c r="D38">
-        <v>0.08783126344801238</v>
+        <v>0.3524878575836192</v>
       </c>
       <c r="E38">
-        <v>0.2185881392297542</v>
+        <v>-0.3994145753096771</v>
       </c>
       <c r="F38">
-        <v>0.9596451603291406</v>
+        <v>-1.772472596017207</v>
       </c>
       <c r="G38">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>CTHRC1,CCL11,SELE,FBLN1,CHI3L1,NOX4,SFRP2,WNT2</t>
+          <t>IL6,INHBA,CXCL8,TESC,ITGA1,THBS1,PTGS2,ACKR3,FLT1,CNN1,CAV2,IL24,WNT5A,PTN,IL1A,VIP</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>GOBP_POSITIVE_REGULATION_OF_MULTICELLULAR_ORGANISMAL_PROCESS</t>
+          <t>GOBP_NEGATIVE_REGULATION_OF_DEVELOPMENTAL_PROCESS</t>
         </is>
       </c>
       <c r="B39">
-        <v>0.9204946996466431</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="C39">
-        <v>0.9567579006772009</v>
+        <v>0.08331131078224101</v>
       </c>
       <c r="D39">
-        <v>0.04380020312998911</v>
+        <v>0.2820133500117251</v>
       </c>
       <c r="E39">
-        <v>-0.1295427578055147</v>
+        <v>-0.3568961457190708</v>
       </c>
       <c r="F39">
-        <v>-0.607248071377379</v>
+        <v>-1.583789568572338</v>
       </c>
       <c r="G39">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>ORM2,ORM1,BAMBI</t>
+          <t>IL6,ANGPT2,GDF15,INHBA,SOX8,SERPINE1,THBS1,SPP1,TNFSF4,SEMA3A,ID4,COL4A2,WNT5A,PTN,IL1A</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>GOBP_POSITIVE_REGULATION_OF_NUCLEOBASE_CONTAINING_COMPOUND_METABOLIC_PROCESS</t>
+          <t>GOBP_NEGATIVE_REGULATION_OF_MULTICELLULAR_ORGANISMAL_PROCESS</t>
         </is>
       </c>
       <c r="B40">
-        <v>0.8324607329842932</v>
+        <v>0.02633225551578239</v>
       </c>
       <c r="C40">
-        <v>0.9567579006772009</v>
+        <v>0.04481103131633144</v>
       </c>
       <c r="D40">
-        <v>0.04782996331142293</v>
+        <v>0.3524878575836192</v>
       </c>
       <c r="E40">
-        <v>-0.1615340429644221</v>
+        <v>-0.3545918948367555</v>
       </c>
       <c r="F40">
-        <v>-0.7053999227491559</v>
+        <v>-1.737015159571814</v>
       </c>
       <c r="G40">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>NEUROD1,BAMBI,SOX8,PKIB,SLC4A4,ID4,KLF4,PLAC8,BMP2,OVOL2,GLYR1,WNT2,SFRP2,CXCL10,NOX4,COL1A1</t>
+          <t>IL6,ANGPT2,FN1,STC1,GDF15,INHBA,SOX8,SERPINE1,THBS1,SPP1,PTGS2,TNFSF4,SEMA3A,ID4,PDGFA,COL4A2,WNT5A,ADAMTS5,PTN</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>GOBP_POSITIVE_REGULATION_OF_PROTEIN_METABOLIC_PROCESS</t>
+          <t>GOBP_NEGATIVE_REGULATION_OF_RESPONSE_TO_STIMULUS</t>
         </is>
       </c>
       <c r="B41">
-        <v>0.9453302961275627</v>
+        <v>0.0002112600790956027</v>
       </c>
       <c r="C41">
-        <v>0.9598738391449098</v>
+        <v>0.001337054783742017</v>
       </c>
       <c r="D41">
-        <v>0.05423159354958409</v>
+        <v>0.5188480777437918</v>
       </c>
       <c r="E41">
-        <v>0.1350292567445855</v>
+        <v>-0.5309734513274337</v>
       </c>
       <c r="F41">
-        <v>0.5759475466184509</v>
+        <v>-2.498758758467395</v>
       </c>
       <c r="G41">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>CYP1B1,C3,FBLN1,CHI3L1,NOX4,SFRP2</t>
+          <t>IL6,ANGPT2,GDF15,NR4A3,CXCL8,SERPINE1,ITGA1,THBS1,SPP1,PTGS2,DKK3,TNFSF4,ACKR3,SEMA3A,PDGFA,LPL,CAV2,WNT5A,PXDN,IL1A</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>GOBP_POSITIVE_REGULATION_OF_SIGNALING</t>
+          <t>GOBP_NEGATIVE_REGULATION_OF_SIGNALING</t>
         </is>
       </c>
       <c r="B42">
-        <v>0.2018561484918794</v>
+        <v>0.001096614291180286</v>
       </c>
       <c r="C42">
-        <v>0.4440835266821346</v>
+        <v>0.004476101044035709</v>
       </c>
       <c r="D42">
-        <v>0.1482615004751066</v>
+        <v>0.4550598673872295</v>
       </c>
       <c r="E42">
-        <v>0.2484333041391171</v>
+        <v>-0.5290536720499223</v>
       </c>
       <c r="F42">
-        <v>1.270246791422073</v>
+        <v>-2.244507601898442</v>
       </c>
       <c r="G42">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>SFRP4,CCL11,CYP1B1,GABBR1,UBD,C3,CHI3L1,COL1A1,NOX4,SFRP2,BST2,CALB1,APELA</t>
+          <t>IL6,IL11,GDF15,BMP8A,INHBA,CXCL8,SERPINE1,ITGA1,THBS1,PTGS2,DKK3,ACKR3</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>GOBP_POSITIVE_REGULATION_OF_TRANSPORT</t>
+          <t>GOBP_NEUROGENESIS</t>
         </is>
       </c>
       <c r="B43">
-        <v>0.3690205011389522</v>
+        <v>0.005307859662744947</v>
       </c>
       <c r="C43">
-        <v>0.5940330018334352</v>
+        <v>0.01320159967400666</v>
       </c>
       <c r="D43">
-        <v>0.1039584715599568</v>
+        <v>0.4070179189239539</v>
       </c>
       <c r="E43">
-        <v>0.2537207587719794</v>
+        <v>-0.4700841851629189</v>
       </c>
       <c r="F43">
-        <v>1.082208789886959</v>
+        <v>-1.994329843779716</v>
       </c>
       <c r="G43">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>SFRP4,CXCL11,SELE,GABBR1,C3,SEC16B,CXCL10</t>
+          <t>IL6,FN1,INHBA,SOX8,ITGA1,SPP1,NTM,MAP1B,SEMA3A,ROBO4,ID4,ANOS1,HECW2</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>GOBP_PROGRAMMED_CELL_DEATH</t>
+          <t>GOBP_NEURON_DIFFERENTIATION</t>
         </is>
       </c>
       <c r="B44">
-        <v>0.3821510297482837</v>
+        <v>0.001107488918111928</v>
       </c>
       <c r="C44">
-        <v>0.6005230467473031</v>
+        <v>0.004476101044035709</v>
       </c>
       <c r="D44">
-        <v>0.1020801076627472</v>
+        <v>0.4550598673872295</v>
       </c>
       <c r="E44">
-        <v>0.202689161278813</v>
+        <v>-0.5390646478822368</v>
       </c>
       <c r="F44">
-        <v>1.063276448322388</v>
+        <v>-2.27516461176372</v>
       </c>
       <c r="G44">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>FAM3B,SFRP4,CYP1B1,FAP,UBD</t>
+          <t>IL6,FN1,INHBA,SOX8,ITGA1,SPP1,NTM,MAP1B,SEMA3A,ROBO4,ID4,ANOS1,HECW2</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>GOBP_PROTEOLYSIS</t>
+          <t>GOBP_PHOSPHORYLATION</t>
         </is>
       </c>
       <c r="B45">
-        <v>0.1670533642691415</v>
+        <v>0.01982952200202923</v>
       </c>
       <c r="C45">
-        <v>0.4083526682134571</v>
+        <v>0.03697999648477727</v>
       </c>
       <c r="D45">
-        <v>0.1644057558382101</v>
+        <v>0.3524878575836192</v>
       </c>
       <c r="E45">
-        <v>0.2577506865381956</v>
+        <v>-0.4190648006659038</v>
       </c>
       <c r="F45">
-        <v>1.317886841687855</v>
+        <v>-1.777880355953603</v>
       </c>
       <c r="G45">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>MMP7,FAP,UBD,MMP13,C3,FBLN1,MMP3,SFRP2,BST2,MMP11,MMP1,MMP2,GAS1,SPOCK1</t>
+          <t>IL6,FN1,IL11,GDF15,BMP8A,INHBA,THBS1,TNFSF11,PTGS2,FLT1,LOX,PDGFA,IL24,WNT5A</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>GOBP_REGULATION_OF_ANATOMICAL_STRUCTURE_MORPHOGENESIS</t>
+          <t>GOBP_POSITIVE_REGULATION_OF_CELLULAR_BIOSYNTHETIC_PROCESS</t>
         </is>
       </c>
       <c r="B46">
-        <v>0.03016557165408999</v>
+        <v>8.573270068136398e-05</v>
       </c>
       <c r="C46">
-        <v>0.183467549888199</v>
+        <v>0.0009003292979184316</v>
       </c>
       <c r="D46">
-        <v>0.3524878575836192</v>
+        <v>0.5384340963099162</v>
       </c>
       <c r="E46">
-        <v>0.365993897956783</v>
+        <v>-0.561362425560763</v>
       </c>
       <c r="F46">
-        <v>1.627340961207407</v>
+        <v>-2.534983451617373</v>
       </c>
       <c r="G46">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>THBS2,CTHRC1,CCL11,CYP1B1,C3,FBLN1,CHI3L1,CXCL10,SFRP2,WNT2,APELA</t>
+          <t>IL6,IL11,INHBA,NR4A3,SOX8,CXCL8,TESC,CREB5,ADGRF5,THBS1,TNFSF11,SPP1,PTGS2</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>GOBP_REGULATION_OF_CELLULAR_COMPONENT_MOVEMENT</t>
+          <t>GOBP_POSITIVE_REGULATION_OF_CELL_ACTIVATION</t>
         </is>
       </c>
       <c r="B47">
-        <v>0.03057792498136649</v>
+        <v>0.2304832713754647</v>
       </c>
       <c r="C47">
-        <v>0.183467549888199</v>
+        <v>0.2599636898072102</v>
       </c>
       <c r="D47">
-        <v>0.3524878575836192</v>
+        <v>0.1215432820354691</v>
       </c>
       <c r="E47">
-        <v>0.3464314739317261</v>
+        <v>0.2852510685704021</v>
       </c>
       <c r="F47">
-        <v>1.679992502785219</v>
+        <v>1.215850057291555</v>
       </c>
       <c r="G47">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>MMP7,CCL11,CYP1B1,SELE,FBLN1,PTPRO,COL1A1,LRRC15,CXCL10,SFRP2,BST2,APELA,MMP2</t>
+          <t>IGLL5,IGKC,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,IGHG2</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>GOBP_REGULATION_OF_CELL_DEATH</t>
+          <t>GOBP_POSITIVE_REGULATION_OF_CELL_POPULATION_PROLIFERATION</t>
         </is>
       </c>
       <c r="B48">
-        <v>0.7958715596330275</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C48">
-        <v>0.9550458715596329</v>
+        <v>0.1947791164658635</v>
       </c>
       <c r="D48">
-        <v>0.06266182309324915</v>
+        <v>0.1608014010700223</v>
       </c>
       <c r="E48">
-        <v>0.1488141564737779</v>
+        <v>-0.2502455367240369</v>
       </c>
       <c r="F48">
-        <v>0.7414646624947144</v>
+        <v>-1.286947302498186</v>
       </c>
       <c r="G48">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>SFRP4,CYP1B1,FAP,UBD</t>
+          <t>ESM1,IL6,FN1,IL11,NR4A3,SOX8,THBS1,PTGS2,CXCL5,TNFSF4,HAS2,FLT1,ID4,PDGFA,CAV2,IL24,WNT5A,PTN,IL1A</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>GOBP_REGULATION_OF_CELL_DIFFERENTIATION</t>
+          <t>GOBP_POSITIVE_REGULATION_OF_DEVELOPMENTAL_PROCESS</t>
         </is>
       </c>
       <c r="B49">
-        <v>0.3459821428571428</v>
+        <v>0.001299490842011413</v>
       </c>
       <c r="C49">
-        <v>0.5809859154929576</v>
+        <v>0.005042024467004284</v>
       </c>
       <c r="D49">
-        <v>0.1067298843646056</v>
+        <v>0.4550598673872295</v>
       </c>
       <c r="E49">
-        <v>0.2023422560487768</v>
+        <v>-0.4440786375200321</v>
       </c>
       <c r="F49">
-        <v>1.087244797776417</v>
+        <v>-2.238012026038876</v>
       </c>
       <c r="G49">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>SFRP4,CTHRC1,CCL11,APOLD1,FBLN1,COL1A1,CXCL10,REG3A,SFRP2,WNT2,HOPX,MMP11,ID3,OVOL2,BMP2,PLA2G10,SPINK5,KLF4,ID4,HES2,ADGRV1,FFAR4</t>
+          <t>IL6,ANGPT2,FN1,GDF15,INHBA,SOX8,CXCL8,SERPINE1,TESC,THBS1,TNFSF11,PTGS2,TNFSF4,MAP1B,HAS2,FLT1,SEMA3A</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>GOBP_REGULATION_OF_CELL_POPULATION_PROLIFERATION</t>
+          <t>GOBP_POSITIVE_REGULATION_OF_GENE_EXPRESSION</t>
         </is>
       </c>
       <c r="B50">
-        <v>0.02537688498917726</v>
+        <v>0.06141364765316171</v>
       </c>
       <c r="C50">
-        <v>0.183467549888199</v>
+        <v>0.09164805880548747</v>
       </c>
       <c r="D50">
-        <v>0.3524878575836192</v>
+        <v>0.3217759180753611</v>
       </c>
       <c r="E50">
-        <v>0.2877803912637987</v>
+        <v>-0.3100034447842508</v>
       </c>
       <c r="F50">
-        <v>1.680493287119511</v>
+        <v>-1.562316623504177</v>
       </c>
       <c r="G50">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>SFRP4,CTHRC1,CCL11,CXCL11,CYP1B1,REG1B,FAP,GABBR1,TNC,FCGR3A,FBLN1,NOX4,CXCL10,REG3A,SFRP2,BST2,CLC,WNT2</t>
+          <t>IL6,FN1,INHBA,NR4A3,SOX8,CXCL8,SERPINE1,TESC,THBS1,TNFSF11,PTGS2,ACTG2,TNFSF4</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>GOBP_REGULATION_OF_HORMONE_LEVELS</t>
+          <t>GOBP_POSITIVE_REGULATION_OF_IMMUNE_RESPONSE</t>
         </is>
       </c>
       <c r="B51">
-        <v>0.7548845470692718</v>
+        <v>0.1463878326996198</v>
       </c>
       <c r="C51">
-        <v>0.9400449076711686</v>
+        <v>0.1739598278335724</v>
       </c>
       <c r="D51">
-        <v>0.05312980547054692</v>
+        <v>0.1585141054248243</v>
       </c>
       <c r="E51">
-        <v>-0.1854604730895678</v>
+        <v>0.3192245604273217</v>
       </c>
       <c r="F51">
-        <v>-0.7648529208968308</v>
+        <v>1.336925106749369</v>
       </c>
       <c r="G51">
         <v>15</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>NEUROD1,SDR16C5,PCSK1,SOX8,CHGA</t>
+          <t>IGLL5,IGKC,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,IGHG2</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>GOBP_REGULATION_OF_HYDROLASE_ACTIVITY</t>
+          <t>GOBP_POSITIVE_REGULATION_OF_IMMUNE_SYSTEM_PROCESS</t>
         </is>
       </c>
       <c r="B52">
-        <v>0.5398633257403189</v>
+        <v>0.5892857142857143</v>
       </c>
       <c r="C52">
-        <v>0.7581059467842777</v>
+        <v>0.6080927051671733</v>
       </c>
       <c r="D52">
-        <v>0.08197787965012722</v>
+        <v>0.07627971808092721</v>
       </c>
       <c r="E52">
-        <v>0.2209326771980765</v>
+        <v>-0.1797585427578094</v>
       </c>
       <c r="F52">
-        <v>0.942356023189624</v>
+        <v>-0.8987616177007898</v>
       </c>
       <c r="G52">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>CCL11,SELE,C3,FBLN1,SFRP2,BST2,SPOCK1,BMP2,TFPI2,SPINK5,PI3,KLF4</t>
+          <t>IL6,NR4A3,COCH,CXCL8,SERPINE1,TESC,THBS1,TNFSF11,TNFSF4,WNT5A,PTN,IL1A,MS4A1,MZB1,IGHG2,IGHV4-31,IGHM,IGHG3,IGHG1,IGHA2,IGHA1</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>GOBP_REGULATION_OF_MULTICELLULAR_ORGANISMAL_DEVELOPMENT</t>
+          <t>GOBP_POSITIVE_REGULATION_OF_INTRACELLULAR_SIGNAL_TRANSDUCTION</t>
         </is>
       </c>
       <c r="B53">
-        <v>0.01442091447926431</v>
+        <v>0.06493506493506493</v>
       </c>
       <c r="C53">
-        <v>0.1427044900199366</v>
+        <v>0.0940104671447955</v>
       </c>
       <c r="D53">
-        <v>0.3807304007227924</v>
+        <v>0.2616635217115731</v>
       </c>
       <c r="E53">
-        <v>0.3667679060167306</v>
+        <v>-0.3395786159010807</v>
       </c>
       <c r="F53">
-        <v>1.875295091488454</v>
+        <v>-1.533458836281151</v>
       </c>
       <c r="G53">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>SFRP4,ASPN,THBS2,CCL11,CYP1B1,APOLD1,C3,CHI3L1,CXCL10,REG3A,SFRP2,WNT2,HOPX,APELA</t>
+          <t>IL6,FN1,IL11,GDF15,ITGA1,THBS1,TNFSF11,ACKR3,FLT1,SEMA3A,PDGFA,CAV2,WNT5A,IL1A,SCHIP1,IQCJ-SCHIP1</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>GOBP_REGULATION_OF_TRANSPORT</t>
+          <t>GOBP_POSITIVE_REGULATION_OF_LOCOMOTION</t>
         </is>
       </c>
       <c r="B54">
-        <v>0.6737089201877934</v>
+        <v>0.02282974750429314</v>
       </c>
       <c r="C54">
-        <v>0.8718586025959679</v>
+        <v>0.03954438406993634</v>
       </c>
       <c r="D54">
-        <v>0.07200331366198796</v>
+        <v>0.3524878575836192</v>
       </c>
       <c r="E54">
-        <v>0.1714216098037198</v>
+        <v>-0.3847573781654517</v>
       </c>
       <c r="F54">
-        <v>0.8119108271103079</v>
+        <v>-1.737475723571622</v>
       </c>
       <c r="G54">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>SFRP4,CXCL11,SELE,GABBR1,C3</t>
+          <t>IL6,FN1,NR4A3,CXCL8,SERPINE1,THBS1,PTGS2,ACKR3,HAS2,FLT1,SEMA3A,MCAM,PDGFA,WNT5A,PTN,IL1A</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>GOBP_REPRODUCTION</t>
+          <t>GOBP_POSITIVE_REGULATION_OF_MAPK_CASCADE</t>
         </is>
       </c>
       <c r="B55">
-        <v>0.8830715532286213</v>
+        <v>0.1470588235294118</v>
       </c>
       <c r="C55">
-        <v>0.9567579006772009</v>
+        <v>0.1739598278335724</v>
       </c>
       <c r="D55">
-        <v>0.04513442222090974</v>
+        <v>0.1669338487131931</v>
       </c>
       <c r="E55">
-        <v>-0.1503646783637748</v>
+        <v>-0.3167181773238038</v>
       </c>
       <c r="F55">
-        <v>-0.6566246380979256</v>
+        <v>-1.336733899691458</v>
       </c>
       <c r="G55">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>SLC26A3,SERPINB5</t>
+          <t>IL6,IL11,GDF15,ITGA1,THBS1,TNFSF11,ACKR3,FLT1,SEMA3A,PDGFA,CAV2,WNT5A,IL1A</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>GOBP_RESPONSE_TO_BACTERIUM</t>
+          <t>GOBP_POSITIVE_REGULATION_OF_MULTICELLULAR_ORGANISMAL_PROCESS</t>
         </is>
       </c>
       <c r="B56">
-        <v>0.9931662870159453</v>
+        <v>0.02028308685529715</v>
       </c>
       <c r="C56">
-        <v>0.9931662870159453</v>
+        <v>0.03697999648477727</v>
       </c>
       <c r="D56">
-        <v>0.05195124761970824</v>
+        <v>0.3524878575836192</v>
       </c>
       <c r="E56">
-        <v>0.1088153887724905</v>
+        <v>-0.3405601671103291</v>
       </c>
       <c r="F56">
-        <v>0.4641361265610454</v>
+        <v>-1.766328193182501</v>
       </c>
       <c r="G56">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>CXCL11,SELE,C3,CCDC80,CXCL10,IFI44,BMP2,SPINK5,PLAC8,PI3</t>
+          <t>IL6,ANGPT2,FN1,INHBA,NR4A3,SOX8,CXCL8,SERPINE1,TESC,THBS1,TNFSF11,PTGS2,TNFSF4,MAP1B,FLT1,SEMA3A</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>GOBP_RESPONSE_TO_CYTOKINE</t>
+          <t>GOBP_POSITIVE_REGULATION_OF_NUCLEOBASE_CONTAINING_COMPOUND_METABOLIC_PROCESS</t>
         </is>
       </c>
       <c r="B57">
-        <v>0.04897390254558952</v>
+        <v>0.008991815052143111</v>
       </c>
       <c r="C57">
-        <v>0.2693564640007424</v>
+        <v>0.01896100130560613</v>
       </c>
       <c r="D57">
-        <v>0.3217759180753611</v>
+        <v>0.3807304007227924</v>
       </c>
       <c r="E57">
-        <v>0.3808468892198795</v>
+        <v>-0.4504155415234052</v>
       </c>
       <c r="F57">
-        <v>1.62444670711893</v>
+        <v>-1.901014107840945</v>
       </c>
       <c r="G57">
         <v>15</v>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>CCL11,CXCL11,CYP1B1,SELE,UBD,CHI3L1,COL1A1,CXCL10,BST2</t>
+          <t>IL6,IL11,INHBA,NR4A3,SOX8,TESC,CREB5,TNFSF11,SPP1,TNFSF4</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>GOBP_RESPONSE_TO_ENDOGENOUS_STIMULUS</t>
+          <t>GOBP_POSITIVE_REGULATION_OF_PHOSPHORUS_METABOLIC_PROCESS</t>
         </is>
       </c>
       <c r="B58">
-        <v>0.5271453590192644</v>
+        <v>0.003890480567815064</v>
       </c>
       <c r="C58">
-        <v>0.7563389933754663</v>
+        <v>0.01109931220817827</v>
       </c>
       <c r="D58">
-        <v>0.06961334388509648</v>
+        <v>0.4317076958033464</v>
       </c>
       <c r="E58">
-        <v>-0.1925788775640282</v>
+        <v>-0.4932935038927349</v>
       </c>
       <c r="F58">
-        <v>-0.937340964609844</v>
+        <v>-2.081983909868376</v>
       </c>
       <c r="G58">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>SLC26A3,CA2,AQP8,BAMBI</t>
+          <t>IL6,IL11,GDF15,BMP8A,INHBA,ITGA1,ADGRF5,THBS1,TNFSF11,PTGS2</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>GOBP_RESPONSE_TO_LIPID</t>
+          <t>GOBP_POSITIVE_REGULATION_OF_PROTEIN_METABOLIC_PROCESS</t>
         </is>
       </c>
       <c r="B59">
-        <v>0.3348729792147806</v>
+        <v>0.01667717177146633</v>
       </c>
       <c r="C59">
-        <v>0.5809859154929576</v>
+        <v>0.03171932670259282</v>
       </c>
       <c r="D59">
-        <v>0.1110114924504503</v>
+        <v>0.3524878575836192</v>
       </c>
       <c r="E59">
-        <v>0.2493982248559732</v>
+        <v>-0.3989330837987434</v>
       </c>
       <c r="F59">
-        <v>1.094907529388655</v>
+        <v>-1.801489946040283</v>
       </c>
       <c r="G59">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>CXCL11,CYP1B1,SELE,FIBIN,COL1A1,CXCL10,WNT2,MMP2,ID3,SCGB2A1,KLF4,PADI2,SST,CXCL5</t>
+          <t>IL6,FN1,IL11,GDF15,BMP8A,INHBA,ITGA1,THBS1,TNFSF11,PTGS2,FLT1,HECW2,PDGFA,IL24,WNT5A</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>GOBP_RESPONSE_TO_NITROGEN_COMPOUND</t>
+          <t>GOBP_POSITIVE_REGULATION_OF_SIGNALING</t>
         </is>
       </c>
       <c r="B60">
-        <v>0.3232682060390764</v>
+        <v>0.008010852808909239</v>
       </c>
       <c r="C60">
-        <v>0.5809859154929576</v>
+        <v>0.01766028914691355</v>
       </c>
       <c r="D60">
-        <v>0.09688777032754396</v>
+        <v>0.3807304007227924</v>
       </c>
       <c r="E60">
-        <v>-0.2720045069848099</v>
+        <v>-0.3490510385773366</v>
       </c>
       <c r="F60">
-        <v>-1.121767016974879</v>
+        <v>-1.888896684498028</v>
       </c>
       <c r="G60">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>SLC26A3,CA2,AQP8</t>
+          <t>ESM1,IL6,FN1,IL11,GDF15,BMP8A,INHBA,ANO1,ITGA1,THBS1,CA2,TNFSF11,SPP1,PTGS2,ACKR3,FLT1,SEMA3A</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>GOBP_RESPONSE_TO_OXYGEN_CONTAINING_COMPOUND</t>
+          <t>GOBP_PRODUCTION_OF_MOLECULAR_MEDIATOR_OF_IMMUNE_RESPONSE</t>
         </is>
       </c>
       <c r="B61">
-        <v>0.565121412803532</v>
+        <v>6.483319949208685e-06</v>
       </c>
       <c r="C61">
-        <v>0.7770419426048565</v>
+        <v>0.0001572205087683106</v>
       </c>
       <c r="D61">
-        <v>0.07788401119770678</v>
+        <v>0.610526878385931</v>
       </c>
       <c r="E61">
-        <v>0.1628689352577293</v>
+        <v>0.6015548434821264</v>
       </c>
       <c r="F61">
-        <v>0.9143847701384442</v>
+        <v>2.78286915599577</v>
       </c>
       <c r="G61">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>CXCL11,CYP1B1,REG1B,SELE,GABBR1,MMP13,FIBIN,COL1A1,NOX4,MMP3,CXCL10,REG3A,WNT2,COL1A2</t>
+          <t>IGKV3D-11,IGLV1-36,IGLV1-44,IGLV1-47,IGKC,IGKV1-16,IGKV1-5,IGKV1D-17,IGKV2-28,IGKV2D-28,CLC,IGKV3-20,IGKV3D-20,IGKV1-12,IGKV1D-12</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>GOBP_SMALL_MOLECULE_METABOLIC_PROCESS</t>
+          <t>GOBP_PROGRAMMED_CELL_DEATH</t>
         </is>
       </c>
       <c r="B62">
-        <v>0.4833040421792619</v>
+        <v>0.1317494600431965</v>
       </c>
       <c r="C62">
-        <v>0.7214780600461893</v>
+        <v>0.1597462203023758</v>
       </c>
       <c r="D62">
-        <v>0.07417589655880091</v>
+        <v>0.1797823162983236</v>
       </c>
       <c r="E62">
-        <v>-0.2172208650339744</v>
+        <v>-0.2801270730015418</v>
       </c>
       <c r="F62">
-        <v>-0.9589532082632407</v>
+        <v>-1.358016043404674</v>
       </c>
       <c r="G62">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>CA1,CA2,SDR16C5,SPTSSB,SLC4A4,GNE,UGT2B15,GCG,DHRS9,CDA,AKR1B10,PLA2G10,BMP2</t>
+          <t>IL6,IL11,INHBA,SOX8,SERPINE1,ITGA1,THBS1,PTGS2,ACKR3,SEMA3A,LOX,IER3,ACTC1,IL24,WNT5A,IL1A,VIP,MZB1,CYP1B1</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>GOBP_TISSUE_DEVELOPMENT</t>
+          <t>GOBP_PROTEOLYSIS</t>
         </is>
       </c>
       <c r="B63">
-        <v>0.005042938122581563</v>
+        <v>0.01618666671936438</v>
       </c>
       <c r="C63">
-        <v>0.08643213275381112</v>
+        <v>0.03140213343556689</v>
       </c>
       <c r="D63">
-        <v>0.4070179189239539</v>
+        <v>0.3524878575836192</v>
       </c>
       <c r="E63">
-        <v>0.3030994548298827</v>
+        <v>-0.4253092607377844</v>
       </c>
       <c r="F63">
-        <v>1.863673636717092</v>
+        <v>-1.795051081326681</v>
       </c>
       <c r="G63">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>SFRP4,ASPN,CTHRC1,CCL11,COL11A1,CYP1B1,APOLD1,TNC,MMP13,C3,PTPRO,CHI3L1,COL1A1,COL12A1,NOX4,CXCL10,REG3A,SFRP2,WNT2,CALB1,HOPX,COL1A2,APELA</t>
+          <t>MMP10,ADAMTS4,FN1,MMP3,MMP1,SERPINE1,THBS1,PTGS2,ENPEP,ANOS1,HECW2,CAPN8</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>GOBP_TISSUE_MORPHOGENESIS</t>
+          <t>GOBP_REGULATION_OF_ANATOMICAL_STRUCTURE_MORPHOGENESIS</t>
         </is>
       </c>
       <c r="B64">
-        <v>0.792147806004619</v>
+        <v>0.007079070953795735</v>
       </c>
       <c r="C64">
-        <v>0.9550458715596329</v>
+        <v>0.01596906703530666</v>
       </c>
       <c r="D64">
-        <v>0.06321911708594577</v>
+        <v>0.4070179189239539</v>
       </c>
       <c r="E64">
-        <v>0.1604104646480222</v>
+        <v>-0.4168943611983097</v>
       </c>
       <c r="F64">
-        <v>0.7412484766254266</v>
+        <v>-2.021044324084774</v>
       </c>
       <c r="G64">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>CTHRC1,CCL11,COL11A1,TNC,CXCL10,SFRP2,WNT2,APELA,MMP2,OVOL2,BMP2,PLA2G10</t>
+          <t>IL6,ANGPT2,FN1,SOX8,COCH,CXCL8,SERPINE1,THBS1,SPP1,MAP1B,HAS2,FLT1,SEMA3A,HECW2,PDGFA,COL4A2,WNT5A,RHOBTB3,IL1A</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>GOBP_TUBE_DEVELOPMENT</t>
+          <t>GOBP_REGULATION_OF_CELLULAR_COMPONENT_MOVEMENT</t>
         </is>
       </c>
       <c r="B65">
-        <v>0.01975639739836058</v>
+        <v>0.003491135733828282</v>
       </c>
       <c r="C65">
-        <v>0.1629902785364748</v>
+        <v>0.01026182321761646</v>
       </c>
       <c r="D65">
-        <v>0.3524878575836192</v>
+        <v>0.4317076958033464</v>
       </c>
       <c r="E65">
-        <v>0.3629227810521933</v>
+        <v>-0.426099352577905</v>
       </c>
       <c r="F65">
-        <v>1.831429040672985</v>
+        <v>-2.0873038715459</v>
       </c>
       <c r="G65">
         <v>22</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>THBS2,CTHRC1,CCL11,CYP1B1,FAP,APOLD1,C3,CHI3L1,CXCL10,SFRP2,WNT2,CALB1,HOPX,APELA,MMP2</t>
+          <t>IL6,ANGPT2,FN1,STC1,NR4A3,CXCL8,SERPINE1,THBS1,PTGS2,ACKR3,HAS2,FLT1,SEMA3A,ROBO4,MCAM,PDGFA,IL24,WNT5A,PTN,IL1A</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>GOBP_TUBE_MORPHOGENESIS</t>
+          <t>GOBP_REGULATION_OF_CELL_ACTIVATION</t>
         </is>
       </c>
       <c r="B66">
-        <v>0.06006898326932115</v>
+        <v>0.388086642599278</v>
       </c>
       <c r="C66">
-        <v>0.3049656073673228</v>
+        <v>0.413674772880549</v>
       </c>
       <c r="D66">
-        <v>0.3217759180753611</v>
+        <v>0.08730982576379309</v>
       </c>
       <c r="E66">
-        <v>0.327121767685039</v>
+        <v>0.2187494653233224</v>
       </c>
       <c r="F66">
-        <v>1.586351583392853</v>
+        <v>1.04676592549274</v>
       </c>
       <c r="G66">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>THBS2,CTHRC1,CCL11,CYP1B1,FAP,APOLD1,C3,CHI3L1,CXCL10,SFRP2,WNT2,APELA,MMP2</t>
+          <t>PLA2G2A,IGLL5,IGKC,CLC,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,IGHG2,MZB1</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
+          <t>GOBP_REGULATION_OF_CELL_ADHESION</t>
+        </is>
+      </c>
+      <c r="B67">
+        <v>0.0005606062040937343</v>
+      </c>
+      <c r="C67">
+        <v>0.002844613730188533</v>
+      </c>
+      <c r="D67">
+        <v>0.4772708153628621</v>
+      </c>
+      <c r="E67">
+        <v>-0.5612458405800197</v>
+      </c>
+      <c r="F67">
+        <v>-2.368782074661662</v>
+      </c>
+      <c r="G67">
+        <v>15</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>IL6,ANGPT2,FN1,NR4A3,CXCL8,SERPINE1,TESC,IBSP,THBS1,TNFSF11,TNFSF4,HAS2</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>GOBP_REGULATION_OF_CELL_DEATH</t>
+        </is>
+      </c>
+      <c r="B68">
+        <v>0.02943883562666025</v>
+      </c>
+      <c r="C68">
+        <v>0.04839944162349227</v>
+      </c>
+      <c r="D68">
+        <v>0.3524878575836192</v>
+      </c>
+      <c r="E68">
+        <v>-0.3756353279964048</v>
+      </c>
+      <c r="F68">
+        <v>-1.737201178434502</v>
+      </c>
+      <c r="G68">
+        <v>19</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>IL6,MMP3,IL11,INHBA,NR4A3,SOX8,SERPINE1,ITGA1,THBS1,PTGS2,ACKR3,LOX,IER3</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>GOBP_REGULATION_OF_CELL_DIFFERENTIATION</t>
+        </is>
+      </c>
+      <c r="B69">
+        <v>0.03304102891364522</v>
+      </c>
+      <c r="C69">
+        <v>0.05169322265521913</v>
+      </c>
+      <c r="D69">
+        <v>0.3217759180753611</v>
+      </c>
+      <c r="E69">
+        <v>-0.3483481271706245</v>
+      </c>
+      <c r="F69">
+        <v>-1.706429240246425</v>
+      </c>
+      <c r="G69">
+        <v>22</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>IL6,FN1,INHBA,SOX8,SERPINE1,TESC,TNFSF11,SPP1,PTGS2,TNFSF4,MAP1B,HAS2,SEMA3A,ID4,LOX</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>GOBP_REGULATION_OF_CELL_POPULATION_PROLIFERATION</t>
+        </is>
+      </c>
+      <c r="B70">
+        <v>0.06741573033707865</v>
+      </c>
+      <c r="C70">
+        <v>0.09616655651024454</v>
+      </c>
+      <c r="D70">
+        <v>0.2616635217115731</v>
+      </c>
+      <c r="E70">
+        <v>-0.2730500330907999</v>
+      </c>
+      <c r="F70">
+        <v>-1.543406013814979</v>
+      </c>
+      <c r="G70">
+        <v>33</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>ESM1,IL6,FN1,IL11,INHBA,NR4A3,SOX8,CXCL8,TESC,ITGA1,THBS1,PTGS2,CXCL5,TNFSF4,ACKR3,HAS2,FLT1,ID4</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>GOBP_REGULATION_OF_IMMUNE_RESPONSE</t>
+        </is>
+      </c>
+      <c r="B71">
+        <v>0.07434944237918216</v>
+      </c>
+      <c r="C71">
+        <v>0.1017651533034333</v>
+      </c>
+      <c r="D71">
+        <v>0.2249660935403137</v>
+      </c>
+      <c r="E71">
+        <v>0.3524979291731734</v>
+      </c>
+      <c r="F71">
+        <v>1.502482109982278</v>
+      </c>
+      <c r="G71">
+        <v>16</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>IGLL5,IGKC,CLC,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,IGHG2</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>GOBP_REGULATION_OF_IMMUNE_SYSTEM_PROCESS</t>
+        </is>
+      </c>
+      <c r="B72">
+        <v>0.6839285714285714</v>
+      </c>
+      <c r="C72">
+        <v>0.6945460085313834</v>
+      </c>
+      <c r="D72">
+        <v>0.05797547575714859</v>
+      </c>
+      <c r="E72">
+        <v>0.1553559877707554</v>
+      </c>
+      <c r="F72">
+        <v>0.8243761728536986</v>
+      </c>
+      <c r="G72">
+        <v>31</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>PLA2G2A,IGLL5,IGKC,ORM1,ORM2,CLC,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,IGHG2</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>GOBP_REGULATION_OF_INTRACELLULAR_SIGNAL_TRANSDUCTION</t>
+        </is>
+      </c>
+      <c r="B73">
+        <v>0.04946878295282488</v>
+      </c>
+      <c r="C73">
+        <v>0.07616622137180974</v>
+      </c>
+      <c r="D73">
+        <v>0.3217759180753611</v>
+      </c>
+      <c r="E73">
+        <v>-0.3512066459135407</v>
+      </c>
+      <c r="F73">
+        <v>-1.624225821381931</v>
+      </c>
+      <c r="G73">
+        <v>19</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>IL6,FN1,IL11,GDF15,ITGA1,THBS1,TNFSF11,PTGS2,ACKR3,FLT1,SEMA3A,PDGFA,CAV2,WNT5A,IL1A,SCHIP1,IQCJ-SCHIP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>GOBP_REGULATION_OF_LYMPHOCYTE_ACTIVATION</t>
+        </is>
+      </c>
+      <c r="B74">
+        <v>0.07357871840751544</v>
+      </c>
+      <c r="C74">
+        <v>0.1017651533034333</v>
+      </c>
+      <c r="D74">
+        <v>0.2878051305355643</v>
+      </c>
+      <c r="E74">
+        <v>0.3797569014909277</v>
+      </c>
+      <c r="F74">
+        <v>1.6186703620381</v>
+      </c>
+      <c r="G74">
+        <v>16</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>IGLL5,IGKC,CLC,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,IGHG2,MZB1</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>GOBP_REGULATION_OF_MULTICELLULAR_ORGANISMAL_DEVELOPMENT</t>
+        </is>
+      </c>
+      <c r="B75">
+        <v>0.004505430092850294</v>
+      </c>
+      <c r="C75">
+        <v>0.01181153294612104</v>
+      </c>
+      <c r="D75">
+        <v>0.4070179189239539</v>
+      </c>
+      <c r="E75">
+        <v>-0.4087697478051944</v>
+      </c>
+      <c r="F75">
+        <v>-2.060066695794697</v>
+      </c>
+      <c r="G75">
+        <v>24</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>IL6,ANGPT2,FN1,INHBA,SOX8,CXCL8,SERPINE1,TESC,THBS1,TNFSF11,SPP1,TNFSF4,MAP1B,FLT1,SEMA3A,ID4,LOX</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>GOBP_REGULATION_OF_PHOSPHORUS_METABOLIC_PROCESS</t>
+        </is>
+      </c>
+      <c r="B76">
+        <v>0.001967341178800336</v>
+      </c>
+      <c r="C76">
+        <v>0.006155874011084922</v>
+      </c>
+      <c r="D76">
+        <v>0.4317076958033464</v>
+      </c>
+      <c r="E76">
+        <v>-0.5066108027169658</v>
+      </c>
+      <c r="F76">
+        <v>-2.248174754178395</v>
+      </c>
+      <c r="G76">
+        <v>17</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>IL6,FN1,IL11,GDF15,BMP8A,INHBA,ITGA1,ADGRF5,THBS1,TNFSF11,PTGS2,FLT1,LOX,PDGFA,IL24,WNT5A</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>GOBP_REGULATION_OF_PROTEIN_MODIFICATION_PROCESS</t>
+        </is>
+      </c>
+      <c r="B77">
+        <v>0.002720312499902958</v>
+      </c>
+      <c r="C77">
+        <v>0.008245947265330841</v>
+      </c>
+      <c r="D77">
+        <v>0.4317076958033464</v>
+      </c>
+      <c r="E77">
+        <v>-0.4985404224875623</v>
+      </c>
+      <c r="F77">
+        <v>-2.115055290687797</v>
+      </c>
+      <c r="G77">
+        <v>16</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>IL6,FN1,IL11,GDF15,BMP8A,INHBA,ITGA1,THBS1,TNFSF11,PTGS2,FLT1,LOX,PDGFA,IL24,WNT5A</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>GOBP_REGULATION_OF_PROTEIN_PHOSPHORYLATION</t>
+        </is>
+      </c>
+      <c r="B78">
+        <v>0.004084798056640669</v>
+      </c>
+      <c r="C78">
+        <v>0.01132072604268985</v>
+      </c>
+      <c r="D78">
+        <v>0.4070179189239539</v>
+      </c>
+      <c r="E78">
+        <v>-0.4901108025707469</v>
+      </c>
+      <c r="F78">
+        <v>-2.068551069399152</v>
+      </c>
+      <c r="G78">
+        <v>15</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>IL6,FN1,IL11,GDF15,BMP8A,INHBA,THBS1,TNFSF11,PTGS2,FLT1,LOX,PDGFA,IL24,WNT5A</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>GOBP_REGULATION_OF_RESPONSE_TO_EXTERNAL_STIMULUS</t>
+        </is>
+      </c>
+      <c r="B79">
+        <v>0.01219620105702555</v>
+      </c>
+      <c r="C79">
+        <v>0.02517088303258464</v>
+      </c>
+      <c r="D79">
+        <v>0.3807304007227924</v>
+      </c>
+      <c r="E79">
+        <v>-0.4314293833100078</v>
+      </c>
+      <c r="F79">
+        <v>-1.914543950832795</v>
+      </c>
+      <c r="G79">
+        <v>17</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>IL6,ANGPT2,MMP3,COCH,CXCL8,SERPINE1,THBS1,TNFSF11,SPP1,PTGS2,TNFSF4,SEMA3A,PDGFA,LPL,WNT5A,PTN</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>GOBP_REGULATION_OF_RESPONSE_TO_STRESS</t>
+        </is>
+      </c>
+      <c r="B80">
+        <v>0.02700789479607293</v>
+      </c>
+      <c r="C80">
+        <v>0.0451683757796392</v>
+      </c>
+      <c r="D80">
+        <v>0.3524878575836192</v>
+      </c>
+      <c r="E80">
+        <v>-0.3727128030582589</v>
+      </c>
+      <c r="F80">
+        <v>-1.753984834282127</v>
+      </c>
+      <c r="G80">
+        <v>20</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>IL6,MMP3,NR4A3,COCH,SERPINE1,THBS1,TNFSF11,SPP1,PTGS2,TNFSF4,ACKR3,SEMA3A,IER3,PDGFA,LPL,WNT5A,PTN,IL1A</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>GOBP_REGULATION_OF_TRANSPORT</t>
+        </is>
+      </c>
+      <c r="B81">
+        <v>9.281745339365276e-05</v>
+      </c>
+      <c r="C81">
+        <v>0.0009003292979184316</v>
+      </c>
+      <c r="D81">
+        <v>0.5384340963099162</v>
+      </c>
+      <c r="E81">
+        <v>-0.5489282137980355</v>
+      </c>
+      <c r="F81">
+        <v>-2.583253792762342</v>
+      </c>
+      <c r="G81">
+        <v>20</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>IL6,IL11,STC1,BMP8A,INHBA,NR4A3,SERPINE1,TESC,ANO1,THBS1,CA2,TNFSF11,SPP1,PTGS2,MAP1B</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>GOBP_REPRODUCTION</t>
+        </is>
+      </c>
+      <c r="B82">
+        <v>0.03240411754729864</v>
+      </c>
+      <c r="C82">
+        <v>0.05152785905062243</v>
+      </c>
+      <c r="D82">
+        <v>0.3217759180753611</v>
+      </c>
+      <c r="E82">
+        <v>-0.3931623931623932</v>
+      </c>
+      <c r="F82">
+        <v>-1.667989519502486</v>
+      </c>
+      <c r="G82">
+        <v>16</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>ANGPT2,STC1,INHBA,SOX8,SPP1,PTGS2,HAS2,SEMA3A,ID4,PDGFA,WNT5A,RHOBTB3,PTN,IL1A,VIP,CYP1B1</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>GOBP_RESPONSE_TO_ABIOTIC_STIMULUS</t>
+        </is>
+      </c>
+      <c r="B83">
+        <v>0.1029411764705882</v>
+      </c>
+      <c r="C83">
+        <v>0.1296791443850267</v>
+      </c>
+      <c r="D83">
+        <v>0.2020717090211599</v>
+      </c>
+      <c r="E83">
+        <v>-0.3418991374158717</v>
+      </c>
+      <c r="F83">
+        <v>-1.443012116073815</v>
+      </c>
+      <c r="G83">
+        <v>15</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>ANGPT2,MMP3,STC1,MMP1,COL11A1,ANO1,THBS1,PTGS2,MAP1B</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>GOBP_RESPONSE_TO_BACTERIUM</t>
+        </is>
+      </c>
+      <c r="B84">
+        <v>0.3170289855072464</v>
+      </c>
+      <c r="C84">
+        <v>0.3416867954911433</v>
+      </c>
+      <c r="D84">
+        <v>0.09923333437711905</v>
+      </c>
+      <c r="E84">
+        <v>0.227220951868785</v>
+      </c>
+      <c r="F84">
+        <v>1.118000363677718</v>
+      </c>
+      <c r="G84">
+        <v>25</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>PLA2G2A,IGLL5,IGKC,JCHAIN,IGKV3-20,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,IGHG2</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>GOBP_RESPONSE_TO_CYTOKINE</t>
+        </is>
+      </c>
+      <c r="B85">
+        <v>0.2133620689655172</v>
+      </c>
+      <c r="C85">
+        <v>0.2434837728194726</v>
+      </c>
+      <c r="D85">
+        <v>0.1380222424966427</v>
+      </c>
+      <c r="E85">
+        <v>-0.2872628028109786</v>
+      </c>
+      <c r="F85">
+        <v>-1.218711028228255</v>
+      </c>
+      <c r="G85">
+        <v>16</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>IL6,CXCL8,THBS1,TNFSF11,PTGS2,CXCL5,ACKR3,HAS2,LOX,IL24,WNT5A,PXDN,IL1A</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>GOBP_RESPONSE_TO_ENDOGENOUS_STIMULUS</t>
+        </is>
+      </c>
+      <c r="B86">
+        <v>0.005776516232854247</v>
+      </c>
+      <c r="C86">
+        <v>0.01400805186467155</v>
+      </c>
+      <c r="D86">
+        <v>0.4070179189239539</v>
+      </c>
+      <c r="E86">
+        <v>-0.377740258692953</v>
+      </c>
+      <c r="F86">
+        <v>-2.028501950321796</v>
+      </c>
+      <c r="G86">
+        <v>28</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>IL6,STC1,GDF15,BMP8A,INHBA,COL4A1,NR4A3,CXCL8,ANO1,THBS1,CA2,SPP1,PTGS2,DKK3,TNFSF4,MAP1B,HAS2,LOX,PDGFA,COL4A2,LPL,CAV2,WNT5A</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>GOBP_RESPONSE_TO_GROWTH_FACTOR</t>
+        </is>
+      </c>
+      <c r="B87">
+        <v>0.0005989373487904391</v>
+      </c>
+      <c r="C87">
+        <v>0.002844613730188533</v>
+      </c>
+      <c r="D87">
+        <v>0.4772708153628621</v>
+      </c>
+      <c r="E87">
+        <v>-0.559322033898305</v>
+      </c>
+      <c r="F87">
+        <v>-2.360662497725376</v>
+      </c>
+      <c r="G87">
+        <v>15</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>ANGPT2,GDF15,BMP8A,CXCL8,IBSP,THBS1,DKK3,MAP1B,HAS2,FLT1,LOX,PDGFA,COL4A2,CAV2,WNT5A</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>GOBP_RESPONSE_TO_HORMONE</t>
+        </is>
+      </c>
+      <c r="B88">
+        <v>0.1096774193548387</v>
+      </c>
+      <c r="C88">
+        <v>0.1363937138130687</v>
+      </c>
+      <c r="D88">
+        <v>0.1978220213151033</v>
+      </c>
+      <c r="E88">
+        <v>-0.3079047509290356</v>
+      </c>
+      <c r="F88">
+        <v>-1.42396749265453</v>
+      </c>
+      <c r="G88">
+        <v>19</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>IL6,STC1,GDF15,INHBA,NR4A3,THBS1,CA2,SPP1,PTGS2,TNFSF4,MAP1B</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>GOBP_RESPONSE_TO_LIPID</t>
+        </is>
+      </c>
+      <c r="B89">
+        <v>0.001474509289387343</v>
+      </c>
+      <c r="C89">
+        <v>0.005396564162215346</v>
+      </c>
+      <c r="D89">
+        <v>0.4550598673872295</v>
+      </c>
+      <c r="E89">
+        <v>-0.476705725738054</v>
+      </c>
+      <c r="F89">
+        <v>-2.243375077269093</v>
+      </c>
+      <c r="G89">
+        <v>20</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>IL6,STC1,INHBA,NR4A3,CXCL8,SERPINE1,TESC,THBS1,SPP1,PTGS2,CXCL5,TNFSF4,MAP1B,LOX,PDGFA,LPL,IL24,WNT5A</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>GOBP_RESPONSE_TO_NITROGEN_COMPOUND</t>
+        </is>
+      </c>
+      <c r="B90">
+        <v>0.09247311827956989</v>
+      </c>
+      <c r="C90">
+        <v>0.1214760018639329</v>
+      </c>
+      <c r="D90">
+        <v>0.2165428367353482</v>
+      </c>
+      <c r="E90">
+        <v>-0.3144148999191152</v>
+      </c>
+      <c r="F90">
+        <v>-1.454074986956713</v>
+      </c>
+      <c r="G90">
+        <v>19</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>IL6,MMP3,STC1,GDF15,COL4A1,NR4A3,ANO1,CA2,PTGS2,TNFSF4,MAP1B</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>GOBP_RESPONSE_TO_OXYGEN_CONTAINING_COMPOUND</t>
+        </is>
+      </c>
+      <c r="B91">
+        <v>0.0008441373462637523</v>
+      </c>
+      <c r="C91">
+        <v>0.003721878299435635</v>
+      </c>
+      <c r="D91">
+        <v>0.4772708153628621</v>
+      </c>
+      <c r="E91">
+        <v>-0.427757847600824</v>
+      </c>
+      <c r="F91">
+        <v>-2.319433961567385</v>
+      </c>
+      <c r="G91">
+        <v>30</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>IL6,ANGPT2,MMP3,STC1,GDF15,INHBA,COL4A1,NR4A3,CXCL8,SERPINE1,TESC,ANO1,THBS1,CA2,SPP1,PTGS2,CXCL5,TNFSF4,MAP1B</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>GOBP_RESPONSE_TO_WOUNDING</t>
+        </is>
+      </c>
+      <c r="B92">
+        <v>0.02058680216678322</v>
+      </c>
+      <c r="C92">
+        <v>0.03697999648477727</v>
+      </c>
+      <c r="D92">
+        <v>0.3524878575836192</v>
+      </c>
+      <c r="E92">
+        <v>-0.4101206010183502</v>
+      </c>
+      <c r="F92">
+        <v>-1.730946152113577</v>
+      </c>
+      <c r="G92">
+        <v>15</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>IL6,FN1,INHBA,SERPINE1,THBS1,SPP1,MAP1B,LOX,MCAM,PDGFA,IL24,WNT5A,PTN,IL1A</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>GOBP_TAXIS</t>
+        </is>
+      </c>
+      <c r="B93">
+        <v>0.001518083206443035</v>
+      </c>
+      <c r="C93">
+        <v>0.005396564162215346</v>
+      </c>
+      <c r="D93">
+        <v>0.4550598673872295</v>
+      </c>
+      <c r="E93">
+        <v>-0.4828210974529129</v>
+      </c>
+      <c r="F93">
+        <v>-2.180308899214686</v>
+      </c>
+      <c r="G93">
+        <v>18</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>IL6,ANGPT2,CXCL8,SERPINE1,ITGA1,THBS1,TNFSF11,CXCL5,ACKR3,FLT1,SEMA3A,ROBO4,ANOS1,LOX,PDGFA</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>GOBP_TISSUE_DEVELOPMENT</t>
+        </is>
+      </c>
+      <c r="B94">
+        <v>0.0006050987599741894</v>
+      </c>
+      <c r="C94">
+        <v>0.002844613730188533</v>
+      </c>
+      <c r="D94">
+        <v>0.4772708153628621</v>
+      </c>
+      <c r="E94">
+        <v>-0.4156006878029038</v>
+      </c>
+      <c r="F94">
+        <v>-2.317353700966623</v>
+      </c>
+      <c r="G94">
+        <v>32</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>IL6,FN1,STC1,BMP8A,INHBA,COL4A1,SOX8,COL11A1,SERPINE1,IBSP,CA2,TNFSF11,SPP1,PTGS2,ACTG2,MAP1B,HAS2,SEMA3A,ROBO4,ID4,LOX,PDGFA,COL4A2,CAV2,ACTC1,WNT5A,PTN,IL1A</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>GOBP_TUBE_DEVELOPMENT</t>
+        </is>
+      </c>
+      <c r="B95">
+        <v>0.0001383943112989868</v>
+      </c>
+      <c r="C95">
+        <v>0.001074015706505882</v>
+      </c>
+      <c r="D95">
+        <v>0.5188480777437918</v>
+      </c>
+      <c r="E95">
+        <v>-0.4853759259748548</v>
+      </c>
+      <c r="F95">
+        <v>-2.517420606220527</v>
+      </c>
+      <c r="G95">
+        <v>26</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>ESM1,IL6,ANGPT2,FN1,COL4A1,SOX8,CXCL8,SERPINE1,ADGRF5,THBS1,PTGS2,ACKR3,HAS2,ENPEP,FLT1,ROBO4,LOX,MCAM,PDGFA,CALD1,COL4A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>GOBP_TUBE_MORPHOGENESIS</t>
+        </is>
+      </c>
+      <c r="B96">
+        <v>4.876255763258238e-05</v>
+      </c>
+      <c r="C96">
+        <v>0.0007079145297453238</v>
+      </c>
+      <c r="D96">
+        <v>0.557332238758646</v>
+      </c>
+      <c r="E96">
+        <v>-0.5180934519366722</v>
+      </c>
+      <c r="F96">
+        <v>-2.664419030766392</v>
+      </c>
+      <c r="G96">
+        <v>25</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>ESM1,IL6,ANGPT2,FN1,COL4A1,SOX8,CXCL8,SERPINE1,ADGRF5,THBS1,PTGS2,ACKR3,HAS2,ENPEP,FLT1,ROBO4,LOX,MCAM,PDGFA,CALD1,COL4A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
           <t>GOBP_VASCULATURE_DEVELOPMENT</t>
         </is>
       </c>
-      <c r="B67">
-        <v>0.005607459431618435</v>
-      </c>
-      <c r="C67">
-        <v>0.08643213275381112</v>
-      </c>
-      <c r="D67">
-        <v>0.4070179189239539</v>
-      </c>
-      <c r="E67">
-        <v>0.4074362378240296</v>
-      </c>
-      <c r="F67">
-        <v>1.929756074658223</v>
-      </c>
-      <c r="G67">
-        <v>19</v>
-      </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>THBS2,CCL11,CYP1B1,FAP,APOLD1,C3,CHI3L1,COL1A1,CXCL10,SFRP2,WNT2,COL1A2,APELA,MMP2</t>
+      <c r="B97">
+        <v>0.0001550125761967252</v>
+      </c>
+      <c r="C97">
+        <v>0.001074015706505882</v>
+      </c>
+      <c r="D97">
+        <v>0.5188480777437918</v>
+      </c>
+      <c r="E97">
+        <v>-0.5063131231392576</v>
+      </c>
+      <c r="F97">
+        <v>-2.551653609943905</v>
+      </c>
+      <c r="G97">
+        <v>24</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>ESM1,IL6,ANGPT2,FN1,COL4A1,CXCL8,SERPINE1,ADGRF5,THBS1,PTGS2,ACKR3,HAS2,ENPEP,FLT1,ROBO4,LOX,MCAM,PDGFA,CALD1,COL4A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>GOBP_VESICLE_MEDIATED_TRANSPORT</t>
+        </is>
+      </c>
+      <c r="B98">
+        <v>0.3062381852551985</v>
+      </c>
+      <c r="C98">
+        <v>0.3337652131433062</v>
+      </c>
+      <c r="D98">
+        <v>0.1039584715599568</v>
+      </c>
+      <c r="E98">
+        <v>0.2619189919461814</v>
+      </c>
+      <c r="F98">
+        <v>1.132491642924709</v>
+      </c>
+      <c r="G98">
+        <v>17</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>IGLL5,IGKC,IGHA1,IGHA2,IGHG1,IGHG3,IGHM,IGHV4-31,IGHG2</t>
         </is>
       </c>
     </row>

</xml_diff>